<commit_message>
Manually correct a few outlier masks that overlapps the edge of the spheres due to bad registration
</commit_message>
<xml_diff>
--- a/databases/3T_NIST_T1maps_database.xlsx
+++ b/databases/3T_NIST_T1maps_database.xlsx
@@ -1900,31 +1900,29 @@
  1361.6 1362.5 1308.2 1326.7 1325.4 1328.8 1332.3 1351.7 1328.4 1300.
  1345.9 1315.8 1261.8 1384.  1321.5 1314.3 1333.8 1341.1 1313.5 1305.9
  1354.  1335.  1345.9 1329.2 1316.  1299.2 1310.9 1320.2 1349.6 1337.2
- 1373.8 1361.9 1331.1 1327.6 1335.2 1361.4]</t>
+ 1361.9 1331.1 1327.6 1335.2 1361.4]</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>[1141.9  943.4  954.3  931.4  925.   934.2 1328.6  932.8  927.8  938.7
-  939.3  945.7  942.4  941.1 5000.   803.7  933.7  939.7  929.8  933.4
-  944.7  933.3  939.1  948.8 1319.2  954.7  949.5  950.9  939.1  936.9
-  946.8  942.6  935.5  949.  1108.7  942.3  947.9  938.4  931.1  937.6
-  943.1  945.4  939.   946.9 1312.   957.7  945.8  931.6  926.   938.1
-  949.4  943.6  927.7  939.3 2532.2  985.3  943.1  936.9  926.5  923.4
-  935.5  945.5  944.1  939.  5000.   856.6  936.4  945.   934.   925.2
-  924.4  923.8  925.1  921.9  999.2  949.8  948.8  938.5  927.3  930.1
-  944.7  817.7  941.9  940.3  935.2  958.7]</t>
+          <t>[943.4 954.3 931.4 925.  934.2 932.8 927.8 938.7 939.3 945.7 942.4 941.1
+ 803.7 933.7 939.7 929.8 933.4 944.7 933.3 939.1 948.8 954.7 949.5 950.9
+ 939.1 936.9 946.8 942.6 935.5 949.  942.3 947.9 938.4 931.1 937.6 943.1
+ 945.4 939.  946.9 957.7 945.8 931.6 926.  938.1 949.4 943.6 927.7 939.3
+ 985.3 943.1 936.9 926.5 923.4 935.5 945.5 944.1 939.  856.6 936.4 945.
+ 934.  925.2 924.4 923.8 925.1 921.9 999.2 949.8 948.8 938.5 927.3 930.1
+ 944.7 817.7 941.9 940.3 935.2 958.7]</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>[653.4 668.8 706.9 654.3 650.8 665.1 696.  677.8 682.5 679.3 671.2 665.4
- 726.7 695.5 668.6 668.4 676.4 673.5 674.8 689.  668.6 883.1 657.5 678.3
- 668.4 672.2 672.4 672.9 671.9 676.9 661.  866.2 647.4 682.4 673.8 679.5
- 674.3 670.2 670.2 670.1 671.  661.  691.8 674.  676.2 669.5 666.8 671.
- 675.4 668.3 648.6 687.1 675.  676.8 677.3 676.8 678.2 679.2 664.8 664.
- 672.  660.2 668.4 672.2 669.7 671.8 677.6 684.4 652.9 678.9 660.2 665.6
- 672.5 673.8 661.6 671.7 653.3 680.5 673.9 677.5 678.  678.9]</t>
+          <t>[668.8 706.9 654.3 650.8 685.  696.  677.8 682.5 679.3 671.2 665.4 664.
+ 668.6 668.4 676.4 673.5 674.8 689.  668.6 655.1 678.3 668.4 672.2 672.4
+ 672.9 671.9 676.9 661.  668.5 682.4 673.8 679.5 674.3 670.2 670.2 670.1
+ 671.  677.  691.8 674.  676.2 669.5 666.8 671.  675.4 668.3 671.4 687.1
+ 675.  676.8 677.3 676.8 678.2 679.2 664.8 671.4 672.  660.2 668.4 672.2
+ 669.7 671.8 677.6 684.4 677.4 678.9 660.2 665.6 672.5 673.8 661.6 671.7
+ 680.5 673.9 677.5 678.  678.9]</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
@@ -3254,16 +3252,13 @@
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>[1965.2 2138.4 1883.7 1886.8 3190.9 1997.1 2008.4 2004.2 2004.6 1960.6
- 2260.6 2712.9 1942.3 1986.  1958.7 1928.9 1946.8 1974.8 1988.2 2309.7
- 3583.9 1989.5 1970.  1980.1 1956.9 1973.4 1994.4 1932.5 1905.5 1948.
- 1814.  1738.8 1913.5 1981.7 1965.8 1914.9 1966.7 1941.6 1909.5 1897.5
- 1934.5 2111.3 3792.6 1908.3 1945.2 1957.9 1927.7 1948.6 1915.6 1950.2
- 1990.4 1996.6 2106.8 3217.2 3106.3 1973.5 1981.9 1986.5 1967.8 1940.3
- 1938.  1962.  1957.6 1956.4 2111.7 1910.9 1969.  1947.7 1959.2 1983.8
- 1955.1 1943.5 1930.7 1965.2 1957.  2348.6 2143.3 2020.8 1971.9 1962.2
- 1945.6 1945.4 1945.9 2017.5 1965.1 2089.7 1985.4 1920.4 1932.  1943.8
- 1980.6 1973.9 2082.6 2041.2 2040.1 2080.6 2044. ]</t>
+          <t>[2008.4 2004.2 2004.6 1960.6 1986.  1958.7 1928.9 1946.8 1974.8 1988.2
+ 1970.  1980.1 1956.9 1973.4 1994.4 1932.5 1905.5 1948.  1981.7 1965.8
+ 1914.9 1966.7 1941.6 1909.5 1897.5 1934.5 1945.2 1957.9 1927.7 1948.6
+ 1915.6 1950.2 1990.4 1996.6 1981.9 1986.5 1967.8 1940.3 1938.  1962.
+ 1957.6 1956.4 1947.7 1959.2 1983.8 1955.1 1943.5 1930.7 1965.2 1957.
+ 2020.8 1971.9 1962.2 1945.6 1945.4 1945.9 2017.5 1985.4 1920.4 1932.
+ 1943.8 1980.6]</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -3304,39 +3299,35 @@
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>[549.1 491.1 487.7 481.8 486.  487.  690.8 489.6 485.4 483.  485.  487.8
- 486.9 487.  350.4 529.5 488.8 487.6 479.7 479.9 487.6 488.9 489.7 489.9
- 819.5 488.7 482.1 488.  483.9 481.8 489.7 492.9 488.7 490.7 723.  492.1
- 484.3 483.  481.4 484.  486.6 488.4 485.  485.7 680.5 496.3 489.7 484.9
- 484.5 489.8 489.9 490.3 491.5 489.5 780.3 492.7 484.7 486.5 490.2 485.8
- 485.1 486.4 487.1 490.9 947.4 511.8 491.1 488.5 493.5 486.7 490.3 490.3
- 485.8 490.8 581.  494.6 487.8 491.1 489.  486.1 488.2 490.3 503.2 494.1
+          <t>[491.1 487.7 481.8 486.  487.  489.6 485.4 483.  485.  487.8 486.9 487.
+ 529.5 488.8 487.6 479.7 479.9 487.6 488.9 489.7 489.9 488.7 482.1 488.
+ 483.9 481.8 489.7 492.9 488.7 490.7 492.1 484.3 483.  481.4 484.  486.6
+ 488.4 485.  485.7 496.3 489.7 484.9 484.5 489.8 489.9 490.3 491.5 489.5
+ 492.7 484.7 486.5 490.2 485.8 485.1 486.4 487.1 490.9 491.1 488.5 493.5
+ 486.7 490.3 490.3 485.8 490.8 494.6 487.8 491.1 489.  486.1 488.2 490.3
  487.7 487.9 486.7 489.5]</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>[ 346.6  335.   332.   328.6  318.   347.1  347.5  342.4  342.   344.7
-  347.   334.2  355.3  346.1  340.1  341.3  341.3  343.5  348.6  348.4
-  341.7  355.7  350.8  340.1  343.3  343.6  345.2  341.7  340.5  343.5
-  348.1  331.6  372.4  348.9  348.1  344.4  341.9  344.5  341.4  340.6
-  342.4  346.8  342.5  355.7  343.9  345.1  342.3  342.4  345.1  344.1
-  342.7  341.   343.9  348.7  355.7  347.3  342.5  343.5  343.6  344.
-  342.2  343.4  343.   343.   349.3 5000.   375.2  349.6  344.5  349.4
-  348.9  346.7  343.   346.   345.2  341.2  517.4  354.5  353.2  346.9
-  344.8  344.   343.2  345.8  346.3  371.   346.7  344.4  341.6  342.4
-  347.6  348.1  360.9  354.9  346.9  342.3  345.6]</t>
+          <t>[347.1 347.5 342.4 342.  344.7 347.  355.3 346.1 340.1 341.3 341.3 343.5
+ 348.6 348.4 341.7 350.8 340.1 343.3 343.6 345.2 341.7 340.5 343.5 348.1
+ 331.6 348.9 348.1 344.4 341.9 344.5 341.4 340.6 342.4 346.8 342.5 343.9
+ 345.1 342.3 342.4 345.1 344.1 342.7 341.  343.9 348.7 347.3 342.5 343.5
+ 343.6 344.  342.2 343.4 343.  343.  349.3 349.6 344.5 349.4 348.9 346.7
+ 343.  346.  345.2 341.2 354.5 353.2 346.9 344.8 344.  343.2 345.8 346.3
+ 346.7 344.4 341.6 342.4 347.6 348.1 346.9 342.3 345.6]</t>
         </is>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>[244.  240.7 240.  242.1 245.2 240.3 242.1 238.1 239.4 239.8 240.  245.4
- 239.  241.5 244.5 241.5 240.9 243.1 242.7 239.2 243.1 241.1 245.2 243.7
- 242.3 241.3 243.4 244.4 243.8 246.1 243.1 244.6 246.5 241.4 240.7 244.2
- 245.7 243.9 246.3 245.3 243.1 242.5 245.9 242.9 241.1 242.9 244.8 241.8
- 243.6 244.2 245.9 244.7 247.1 246.8 245.  243.1 244.8 245.  244.9 244.7
- 246.1 242.5 245.3 247.8 245.7 244.9 244.4 246.5 246.9 245.6 245.  244.6
- 248.  245.6 248.1 247.1 246.7 248.  247.9 242.9 244.7 251.3 250.  243.5]</t>
+          <t>[244.  240.7 240.  242.1 245.2 240.3 242.1 238.1 239.4 239.8 240.  239.
+ 241.5 244.5 241.5 240.9 243.1 242.7 239.2 243.1 241.1 245.2 243.7 242.3
+ 241.3 243.4 244.4 243.8 246.1 243.1 244.6 246.5 241.4 240.7 244.2 245.7
+ 243.9 246.3 245.3 243.1 242.5 245.9 242.9 241.1 242.9 244.8 241.8 243.6
+ 244.2 245.9 244.7 247.1 246.8 245.  243.1 244.8 245.  244.9 244.7 242.5
+ 245.3 247.8 245.7 244.9 244.4 246.5 246.9 245.6 245.  244.6 248.  245.6
+ 248.1 247.1 246.7 248.  247.9 242.9 244.7 251.3 250.  243.5]</t>
         </is>
       </c>
       <c r="AK11" t="inlineStr">
@@ -8080,11 +8071,10 @@
           <t>[170.8 241.2 234.1  72.1  63.4  97.6 105.2 224.9 208.7   3.    3.    2.1
   82.   94.3  74.3  56.4   1.   86.7   2.    5.3   4.1  80.7  82.1  87.4
   97.   82.7  77.6  80.6   1.3  56.5  60.3  63.5  86.1  77.8  79.9   2.1
-   1.2   3.2   1.3  56.7  85.1  78.    9.5   1.1   3.3  78.6 214.  186.
-  72.5  82.2   3.3   3.2  79.5   2.1  76.7  76.6 103.3  66.  144.5  97.8
-  85.6 144.5  82.3  87.8  87.7   3.  171.5 129.7   4.   82.1  95.  243.7
-  66.2  92.5 692.7 315.3 255.6 191.1  98.9 181.    1.   71.4 121.5  92.3
-   1.8   4.2 116.1   2.7   2.7]</t>
+   1.2   3.2   1.3  56.7  85.1  78.    9.5   1.1   3.3  78.6 186.   72.5
+  82.2   3.3   3.2  79.5   2.1  76.7  76.6 103.3  66.  144.5  97.8  85.6
+ 144.5  82.3  87.8  87.7   3.    4.   82.1  95.  243.7  66.2  92.5 692.7
+ 191.1  98.9 181.    1.   71.4]</t>
         </is>
       </c>
     </row>
@@ -8331,22 +8321,12 @@
       </c>
       <c r="AO29" t="inlineStr">
         <is>
-          <t>[1.1600e+02 1.2010e+02 1.3270e+02 1.1980e+02 1.2000e+00 9.3300e+01
- 1.2000e+00 6.0000e+01 9.3900e+01 1.3290e+02 1.4240e+02 1.5560e+02
- 5.0000e+03 6.1200e+01 9.9900e+01 7.1500e+01 1.0650e+02 1.0670e+02
- 1.2380e+02 5.0500e+01 5.3150e+02 9.6430e+02 1.3320e+02 1.0400e+02
- 1.0290e+02 1.1370e+02 9.4300e+01 1.5320e+02 1.3240e+02 3.5150e+02
- 1.1840e+02 1.1090e+02 8.9900e+01 1.0190e+02 9.9800e+01 1.0530e+02
- 1.2030e+02 1.0050e+02 1.3590e+02 1.2000e+00 2.1350e+02 3.9590e+02
- 2.1010e+02 8.1700e+01 8.1400e+01 1.0230e+02 1.0100e+02 1.2510e+02
- 7.5700e+01 1.4550e+02 3.2000e+00 3.5000e+00 2.4030e+02 1.0575e+03
- 9.6800e+01 9.5800e+01 9.9200e+01 9.8900e+01 1.1860e+02 7.0900e+01
- 1.3860e+02 2.4000e+00 1.2000e+00 2.6520e+02 4.6000e+00 1.0930e+02
- 9.9300e+01 8.9000e+01 1.0130e+02 9.6300e+01 1.1320e+02 9.5000e+00
- 1.2000e+00 1.5750e+02 2.3310e+02 8.2000e+01 7.3000e+01 8.5700e+01
- 9.4200e+01 8.3400e+01 2.0000e+00 5.9200e+01 3.7200e+01 1.1160e+02
- 8.4800e+01 8.7300e+01 9.9800e+01 9.8700e+01 9.3800e+01 7.9600e+01
- 5.5600e+01 8.1800e+01 7.7100e+01 8.7700e+01]</t>
+          <t>[ 93.3   1.2  60.   93.9 132.9  61.2  99.9  71.5 106.5 106.7 123.8 133.2
+ 104.  102.9 113.7  94.3 153.2  89.9 101.9  99.8 105.3 120.3 100.5 135.9
+   1.2  81.7  81.4 102.3 101.  125.1  75.7 145.5   3.2  96.8  95.8  99.2
+  98.9 118.6  70.9 138.6   2.4   1.2 109.3  99.3  89.  101.3  96.3 113.2
+   9.5   1.2  82.   73.   85.7  94.2  83.4   2.   59.2  37.2  84.8  87.3
+  99.8  98.7  93.8  79.6  55.6  81.8  77.1  87.7]</t>
         </is>
       </c>
       <c r="AP29" t="inlineStr">
@@ -8613,15 +8593,14 @@
       </c>
       <c r="AO30" t="inlineStr">
         <is>
-          <t>[ 169.  1860.9  420.   145.   195.3  167.8  177.6  181.2 2513.  1345.2
-   98.3  191.7   15.   170.   157.2  153.4  124.5 1180.8 5000.   251.9
-  202.4    9.5  145.8  142.1  136.7  162.7  168.8  210.5   71.4  257.2
-  179.   134.9  130.5  161.7  131.6  133.3  145.3  132.6  137.7  159.4
-  153.   156.2  120.9  117.7  137.3  135.8  163.1  148.   126.3  138.7
-  126.1  134.9  159.   153.1  125.6  115.8  123.5  136.2  156.2  129.
-  131.2  128.3  140.5  171.   106.   131.5  131.8  123.4  133.1  124.5
-  155.2  110.4  139.6  156.9  134.1  124.2  144.9  105.8  130.5  147.
-  142.2  125.9  125.7  151.7  125.7  142.4  134.6]</t>
+          <t>[1860.9  167.8  177.6  181.2 2513.   191.7   15.   170.   157.2  153.4
+  202.4    9.5  145.8  142.1  136.7  162.7   71.4  257.2  179.   134.9
+  130.5  161.7  131.6  133.3  137.7  159.4  153.   156.2  120.9  117.7
+  137.3  135.8  163.1  148.   126.3  138.7  126.1  134.9  159.   153.1
+  125.6  115.8  123.5  136.2  156.2  129.   131.2  128.3  140.5  171.
+  106.   131.5  131.8  123.4  133.1  124.5  155.2  110.4  139.6  156.9
+  134.1  124.2  144.9  105.8  130.5  147.   142.2  125.9  125.7  151.7
+  125.7  142.4  134.6]</t>
         </is>
       </c>
       <c r="AP30" t="inlineStr">
@@ -8644,8 +8623,8 @@
  256.5 213.2 258.3 256.6 302.6 325.  347.6 259.9 292.1 276.8 286.2 253.5
  301.4 264.9 263.8 454.3 284.5 338.6 371.7 311.4 253.1 224.8 263.1 299.9
  207.  305.8 350.1 290.4 245.1 290.9 347.8 338.9 286.6 219.5 260.9 369.4
- 293.9 470.2 343.8 270.9 242.7 218.6 251.2 347.1 381.5 229.1 314.1 436.2
- 422.7 430.2 413.2 307.5 116.6 332.7 248.9 251.  122.3 119.9]</t>
+ 470.2 343.8 270.9 242.7 218.6 251.2 347.1 381.5 314.1 436.2 422.7 430.2
+ 413.2 307.5]</t>
         </is>
       </c>
     </row>
@@ -8886,22 +8865,19 @@
  107.  118.1 113.1 114.3 114.1 136.5 140.8 126.2 122.6 112.3 116.  111.4
  107.5 108.8 118.3 109.  138.3 140.1 127.  133.8 116.6 110.7 107.1 112.6
  116.6 122.7 116.7 153.8 131.7 135.8 109.9 128.  102.7 119.5 114.1 124.7
- 118.8 125.7 189.4 119.6 144.7 108.4 125.2 121.1 119.2 119.  121.5 119.6
- 114.7 145.2 132.  114.4 115.7 121.6 117.6 126.9 121.6 161.2 121.  133.3
- 140.1 124.7 118.3 118.7 120.  110.1 126.1 137.2 135.7 130.4]</t>
+ 118.8 125.7 119.6 144.7 108.4 125.2 121.1 119.2 119.  121.5 119.6 114.7
+ 145.2 132.  114.4 115.7 121.6 117.6 126.9 121.6 121.  133.3 140.1 124.7
+ 118.3 118.7 120.  110.1 126.1 137.2 135.7 130.4]</t>
         </is>
       </c>
       <c r="AO31" t="inlineStr">
         <is>
-          <t>[ 250.8  137.3  172.5  151.5  168.1  174.5 1837.3  293.7  136.3  175.4
-   10.   159.6  150.4  159.2  722.9  283.5  179.1  176.2   13.   138.2
-  127.9  131.7  163.1  153.9  206.2  122.3  252.7  181.9    9.5  130.3
-  148.6  122.5  177.9  119.   167.3  150.7  170.8  149.4   13.   126.4
-  130.4  143.4  131.8  173.   138.5  168.8  150.4  146.4  143.3  143.
-  139.4  127.5  115.6  135.5  183.4  144.8  139.6  127.3  145.8  159.4
-  105.3  143.4  123.4  110.1  151.7  124.8  142.9  127.   143.1  149.
-  149.4  128.1  129.4  107.5  140.2  154.   137.2  129.4  136.8  156.2
-  172.3  140.8  145.1]</t>
+          <t>[172.5 151.5 168.1 136.3 175.4  10.  159.6 150.4 179.1 176.2  13.  138.2
+ 127.9 131.7 122.3 252.7 181.9   9.5 130.3 148.6 122.5 177.9 119.  167.3
+ 150.7 170.8 149.4  13.  126.4 130.4 143.4 131.8 173.  138.5 168.8 150.4
+ 146.4 143.3 143.  139.4 127.5 115.6 135.5 183.4 144.8 139.6 127.3 145.8
+ 159.4 105.3 143.4 123.4 110.1 151.7 124.8 142.9 127.  143.1 149.  149.4
+ 128.1 129.4 107.5 140.2 154.  137.2 129.4 136.8 156.2 172.3 140.8 145.1]</t>
         </is>
       </c>
       <c r="AP31" t="inlineStr">
@@ -8923,8 +8899,8 @@
  244.7 207.3 212.7 272.6 453.5 288.3 290.1 244.3 273.2 206.2 192.8 240.2
  245.4 255.5 247.8 506.  305.8 257.3 255.4 245.7 250.9 268.7 244.6 284.1
  263.1 265.9 421.1 247.  260.4 252.9 226.4 216.2 240.7 278.7 207.7 320.3
- 469.8 432.9 293.6 265.8 290.  319.9 263.5 249.  284.4 404.4 423.1 382.1
- 299.2 277.6 280.3 362.  362.7 297.9 358.  396.  448.7 412.5]</t>
+ 469.8 432.9 293.6 265.8 290.  319.9 263.5 249.  284.4 423.1 382.1 299.2
+ 277.6 280.3 362. ]</t>
         </is>
       </c>
     </row>

</xml_diff>